<commit_message>
fixing example in supplementary materials
</commit_message>
<xml_diff>
--- a/examples/genomics/schema_and_data.xlsx
+++ b/examples/genomics/schema_and_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22770" windowHeight="10800"/>
+    <workbookView windowWidth="22770" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>!!!ObjTables objTablesVersion='1.0.1' date='2020-05-14 17:04:33'</t>
   </si>
@@ -100,6 +100,15 @@
     <t>Id</t>
   </si>
   <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
@@ -109,15 +118,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
     <t>Transcript</t>
   </si>
   <si>
@@ -145,13 +145,16 @@
     <t>five_prime</t>
   </si>
   <si>
+    <t>PositiveInteger(primary=True, unique=True)</t>
+  </si>
+  <si>
+    <t>5'</t>
+  </si>
+  <si>
+    <t>three_prime</t>
+  </si>
+  <si>
     <t>PositiveInteger</t>
-  </si>
-  <si>
-    <t>5'</t>
-  </si>
-  <si>
-    <t>three_prime</t>
   </si>
   <si>
     <t>3'</t>
@@ -219,10 +222,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -254,8 +257,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,7 +289,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,24 +333,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,44 +372,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,29 +392,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -423,13 +426,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,25 +510,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,61 +540,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,73 +600,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,17 +620,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,11 +659,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,22 +678,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -717,142 +720,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1231,7 +1234,7 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -1319,7 +1322,7 @@
   <sheetPr/>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -1468,7 +1471,7 @@
     </row>
     <row r="8" customHeight="1" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>22</v>
@@ -1477,17 +1480,17 @@
         <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" customHeight="1" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>22</v>
@@ -1496,17 +1499,17 @@
         <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" customHeight="1" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>22</v>
@@ -1518,14 +1521,14 @@
         <v>34</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" customHeight="1" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -1535,7 +1538,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -1550,10 +1553,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>38</v>
@@ -1569,7 +1572,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>40</v>
@@ -1588,13 +1591,13 @@
         <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1632,7 +1635,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1643,41 +1646,41 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6">
         <v>44905791</v>
@@ -1688,13 +1691,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6">
         <v>32315086</v>
@@ -1752,7 +1755,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1763,41 +1766,41 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6">
         <v>44905796</v>
@@ -1808,13 +1811,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6">
         <v>32315474</v>
@@ -1825,13 +1828,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6">
         <v>44906360</v>
@@ -1842,13 +1845,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6">
         <v>32315480</v>

</xml_diff>